<commit_message>
Desarrollo obtener y buscar productos
Desarrollo obtener y buscar productos
</commit_message>
<xml_diff>
--- a/Challenge/Data/Config.xlsx
+++ b/Challenge/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/alexandra_veizu_uipath_com/Documents/Documents/Projects/REFrameworkNET5/StudioTemplates/REFramework/contentFiles/any/any/pt2/VisualBasic/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desktop - 6003 0431\Documents\Uipath\Challenge\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8C54E24-BA5C-4BF9-8DAB-2778512EC11B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD067EDA-01AF-4567-9941-0F7A66E236E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="63">
   <si>
     <t>Name</t>
   </si>
@@ -85,9 +85,6 @@
   </si>
   <si>
     <t>logF_BusinessProcessName</t>
-  </si>
-  <si>
-    <t>Framework</t>
   </si>
   <si>
     <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
@@ -98,75 +95,131 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
+    <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with a system exception. Must be an integer value.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction succesful.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction failed with business exception.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction failed with application exception.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Calling Get Transaction Data.</t>
+  </si>
+  <si>
+    <t>OrchestratorAssetFolder</t>
+  </si>
+  <si>
+    <t>OrchestratorQueueFolder</t>
+  </si>
+  <si>
+    <t>Folder name. The value must match a folder defined in Orchestrator and queue specified as OrchestratorQueueName should be created in this folder. For classic folders leave the value field empty.</t>
+  </si>
+  <si>
+    <t>MaxConsecutiveSystemExceptions</t>
+  </si>
+  <si>
+    <t>ExceptionMessage_ConsecutiveErrors</t>
+  </si>
+  <si>
+    <t>RetryNumberGetTransactionItem</t>
+  </si>
+  <si>
+    <t>RetryNumberSetTransactionStatus</t>
+  </si>
+  <si>
+    <t>Error message in case MaxConsecutiveSystemExceptions number is reached.</t>
+  </si>
+  <si>
+    <t>The number of times Get Transaction Item activity is retried in case of an exception. Must be an integer &gt;= 1.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of times Set transaction status activity is retried in case of an exception. Must be an integer &gt;= 1. </t>
+  </si>
+  <si>
+    <t>ShouldMarkJobAsFaulted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of consecutive system exceptions allowed. If MaxConsecutiveSystemExceptions is reached, the job is stopped. To disable this feature, set the value to 0. </t>
+  </si>
+  <si>
+    <t>Must be TRUE or FALSE. If the value is TRUE and an error occurs in Initialization state or the MaxConsecutiveSystemExceptions is reached, the job is marked as Faulted.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
+  </si>
+  <si>
+    <t>Felipe's Folder</t>
+  </si>
+  <si>
+    <t>Productos</t>
+  </si>
+  <si>
+    <t>Challenge Final</t>
+  </si>
+  <si>
+    <t>Excel</t>
+  </si>
+  <si>
+    <t>EDGE</t>
+  </si>
+  <si>
+    <t>Navegador</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nombre del ejecutable del navegador </t>
+  </si>
+  <si>
+    <t>UrlAmazon</t>
+  </si>
+  <si>
+    <t>C:\Users\Desktop - 6003 0431\Documents\Challenge\Challenge RPA - NI - Productos.pdf</t>
+  </si>
+  <si>
+    <t>RutaInsumoPDF</t>
+  </si>
+  <si>
+    <t>Ruta archivo insumo</t>
+  </si>
+  <si>
+    <t>PDF</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/</t>
+  </si>
+  <si>
+    <t>Url Sitio web amazon</t>
+  </si>
+  <si>
+    <t>RutaPlantilla</t>
+  </si>
+  <si>
     <t>OrchestratorQueueName</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with a system exception. Must be an integer value.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction succesful.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction failed with business exception.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction failed with application exception.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Calling Get Transaction Data.</t>
-  </si>
-  <si>
-    <t>OrchestratorAssetFolder</t>
-  </si>
-  <si>
-    <t>OrchestratorQueueFolder</t>
-  </si>
-  <si>
-    <t>Folder name. The value must match a folder defined in Orchestrator and queue specified as OrchestratorQueueName should be created in this folder. For classic folders leave the value field empty.</t>
-  </si>
-  <si>
-    <t>MaxConsecutiveSystemExceptions</t>
-  </si>
-  <si>
-    <t>ExceptionMessage_ConsecutiveErrors</t>
-  </si>
-  <si>
-    <t>RetryNumberGetTransactionItem</t>
-  </si>
-  <si>
-    <t>RetryNumberSetTransactionStatus</t>
-  </si>
-  <si>
-    <t>Error message in case MaxConsecutiveSystemExceptions number is reached.</t>
-  </si>
-  <si>
-    <t>The number of times Get Transaction Item activity is retried in case of an exception. Must be an integer &gt;= 1.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of times Set transaction status activity is retried in case of an exception. Must be an integer &gt;= 1. </t>
-  </si>
-  <si>
-    <t>ShouldMarkJobAsFaulted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of consecutive system exceptions allowed. If MaxConsecutiveSystemExceptions is reached, the job is stopped. To disable this feature, set the value to 0. </t>
-  </si>
-  <si>
-    <t>Must be TRUE or FALSE. If the value is TRUE and an error occurs in Initialization state or the MaxConsecutiveSystemExceptions is reached, the job is marked as Faulted.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
-  </si>
-  <si>
-    <t>ProcessABCQueue</t>
+  </si>
+  <si>
+    <t>Data\Input\Challenge RPA - NI - InOut - Template.xlsx</t>
+  </si>
+  <si>
+    <t>Ruta de archivo de entrada plantilla</t>
+  </si>
+  <si>
+    <t>RutaFinalArchivpChallenge</t>
+  </si>
+  <si>
+    <t>Data\Out\Challenge RPA - NI - InOut - Template.xlsx</t>
+  </si>
+  <si>
+    <t>Microsoft Edge.exe</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -190,13 +243,38 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -208,21 +286,27 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+  <cellXfs count="7">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -239,9 +323,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -279,7 +363,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -385,7 +469,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -527,7 +611,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -537,11 +621,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="43.5546875" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
@@ -585,22 +669,24 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="43.2">
       <c r="A3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" s="2"/>
+        <v>29</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="C3" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
@@ -609,39 +695,107 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+    </row>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" t="s">
+        <v>61</v>
+      </c>
+    </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" ht="14.25" customHeight="1"/>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1"/>
-    <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A16" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+    </row>
+    <row r="17" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A17" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="20" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -1609,9 +1763,17 @@
     <row r="997" ht="14.25" customHeight="1"/>
     <row r="998" ht="14.25" customHeight="1"/>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A16:D16"/>
+  </mergeCells>
   <phoneticPr fontId="2"/>
+  <hyperlinks>
+    <hyperlink ref="B12" r:id="rId1" xr:uid="{BE4E6546-CD69-4033-BF3C-A67F925C3B93}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1620,10 +1782,10 @@
   <dimension ref="A1:Z988"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
@@ -1673,18 +1835,18 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="43.2">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1708,7 +1870,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -1730,7 +1892,7 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -1741,7 +1903,7 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
@@ -1752,53 +1914,53 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" spans="1:3" ht="28.8">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B17" t="b">
         <v>0</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2782,9 +2944,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="31.88671875" customWidth="1"/>
     <col min="2" max="2" width="30.109375" customWidth="1"/>
@@ -2800,7 +2962,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>

</xml_diff>